<commit_message>
Modify ch9 no optimize
</commit_message>
<xml_diff>
--- a/Ch9/9.10/performance.xlsx
+++ b/Ch9/9.10/performance.xlsx
@@ -1528,7 +1528,7 @@
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" workbookViewId="0">
-      <selection activeCell="I5" sqref="A1:I5"/>
+      <selection activeCell="B3" sqref="B3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,11 +1609,11 @@
         <v>4</v>
       </c>
       <c r="B3" s="7">
-        <f>B7 * B6 / B1 + LOG(B1, 2) * B8</f>
+        <f>B7 * B6 * 2^ (B6 / 2) / B1</f>
         <v>1.3423824788000001</v>
       </c>
       <c r="C3" s="7">
-        <f t="shared" ref="C3:I3" si="0">C7 * C6 / C1 + LOG(C1, 2) * C8</f>
+        <f t="shared" ref="C3:I3" si="0">C7 * C6 * 2^ (C6 / 2) / C1</f>
         <v>0.67119123940000003</v>
       </c>
       <c r="D3" s="7">
@@ -1717,28 +1717,28 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>1000000</v>
+        <v>50</v>
       </c>
       <c r="C6">
-        <v>1000000</v>
+        <v>50</v>
       </c>
       <c r="D6">
-        <v>1000000</v>
+        <v>50</v>
       </c>
       <c r="E6">
-        <v>1000000</v>
+        <v>50</v>
       </c>
       <c r="F6">
-        <v>1000000</v>
+        <v>50</v>
       </c>
       <c r="G6">
-        <v>1000000</v>
+        <v>50</v>
       </c>
       <c r="H6">
-        <v>1000000</v>
+        <v>50</v>
       </c>
       <c r="I6">
-        <v>1000000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1746,36 +1746,36 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <f>B2/B6</f>
-        <v>1.3423824788E-6</v>
+        <f>B2/(B6 * 2^(B6 / 2))</f>
+        <v>8.0012230801582344E-10</v>
       </c>
       <c r="C7">
         <f>B7</f>
-        <v>1.3423824788E-6</v>
+        <v>8.0012230801582344E-10</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:I7" si="2">C7</f>
-        <v>1.3423824788E-6</v>
+        <v>8.0012230801582344E-10</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>1.3423824788E-6</v>
+        <v>8.0012230801582344E-10</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>1.3423824788E-6</v>
+        <v>8.0012230801582344E-10</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>1.3423824788E-6</v>
+        <v>8.0012230801582344E-10</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>1.3423824788E-6</v>
+        <v>8.0012230801582344E-10</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>1.3423824788E-6</v>
+        <v>8.0012230801582344E-10</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add ch9 report & modified ch6
</commit_message>
<xml_diff>
--- a/Ch9/9.10/performance.xlsx
+++ b/Ch9/9.10/performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -255,28 +255,28 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.3423824788000001</c:v>
+                  <c:v>2.1521389480000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67520730490000003</c:v>
+                  <c:v>1.085650921</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47397558690000002</c:v>
+                  <c:v>0.72222399699999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35781226160000001</c:v>
+                  <c:v>0.53893685300000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28761031640000001</c:v>
+                  <c:v>0.434614897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23953547480000001</c:v>
+                  <c:v>0.372735977</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.20902197380000001</c:v>
+                  <c:v>0.31239581100000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1829732657</c:v>
+                  <c:v>0.27757406200000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -333,28 +333,28 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.3423824788000001</c:v>
+                  <c:v>2.1521389480000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.67119123940000003</c:v>
+                  <c:v>1.0760694740000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.44746082626666667</c:v>
+                  <c:v>0.71737964933333342</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33559561970000001</c:v>
+                  <c:v>0.53803473700000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.26847649575999999</c:v>
+                  <c:v>0.43042778960000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.22373041313333333</c:v>
+                  <c:v>0.35868982466666671</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.19176892554285715</c:v>
+                  <c:v>0.30744842114285714</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16779780985000001</c:v>
+                  <c:v>0.26901736850000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1528,7 +1528,7 @@
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:I3"/>
+      <selection sqref="A1:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,28 +1580,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="7">
-        <v>1.3423824788000001</v>
+        <v>2.1521389480000002</v>
       </c>
       <c r="C2" s="7">
-        <v>0.67520730490000003</v>
+        <v>1.085650921</v>
       </c>
       <c r="D2" s="7">
-        <v>0.47397558690000002</v>
+        <v>0.72222399699999995</v>
       </c>
       <c r="E2" s="7">
-        <v>0.35781226160000001</v>
+        <v>0.53893685300000005</v>
       </c>
       <c r="F2" s="7">
-        <v>0.28761031640000001</v>
+        <v>0.434614897</v>
       </c>
       <c r="G2" s="7">
-        <v>0.23953547480000001</v>
+        <v>0.372735977</v>
       </c>
       <c r="H2" s="7">
-        <v>0.20902197380000001</v>
+        <v>0.31239581100000002</v>
       </c>
       <c r="I2" s="7">
-        <v>0.1829732657</v>
+        <v>0.27757406200000001</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1610,35 +1610,35 @@
       </c>
       <c r="B3" s="7">
         <f>B7 * B6 * 2^ (B6 / 2) / B1</f>
-        <v>1.3423824788000001</v>
+        <v>2.1521389480000002</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" ref="C3:I3" si="0">C7 * C6 * 2^ (C6 / 2) / C1</f>
-        <v>0.67119123940000003</v>
+        <v>1.0760694740000001</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" si="0"/>
-        <v>0.44746082626666667</v>
+        <v>0.71737964933333342</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" si="0"/>
-        <v>0.33559561970000001</v>
+        <v>0.53803473700000004</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" si="0"/>
-        <v>0.26847649575999999</v>
+        <v>0.43042778960000005</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" si="0"/>
-        <v>0.22373041313333333</v>
+        <v>0.35868982466666671</v>
       </c>
       <c r="H3" s="7">
         <f t="shared" si="0"/>
-        <v>0.19176892554285715</v>
+        <v>0.30744842114285714</v>
       </c>
       <c r="I3" s="7">
         <f t="shared" si="0"/>
-        <v>0.16779780985000001</v>
+        <v>0.26901736850000002</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1651,31 +1651,31 @@
       </c>
       <c r="C4" s="7">
         <f>B2/C2</f>
-        <v>1.9881042000853506</v>
+        <v>1.9823489358970479</v>
       </c>
       <c r="D4" s="7">
         <f>B2/D2</f>
-        <v>2.8321764156245828</v>
+        <v>2.9798773745259539</v>
       </c>
       <c r="E4" s="7">
         <f>B2/E2</f>
-        <v>3.7516391215811815</v>
+        <v>3.9933044771759185</v>
       </c>
       <c r="F4" s="7">
         <f>B2/F2</f>
-        <v>4.6673655368225866</v>
+        <v>4.9518296838315692</v>
       </c>
       <c r="G4" s="7">
         <f>B2/G2</f>
-        <v>5.6041071992397846</v>
+        <v>5.77389648652027</v>
       </c>
       <c r="H4" s="7">
         <f>B2/H2</f>
-        <v>6.4222074569271914</v>
+        <v>6.8891415064461281</v>
       </c>
       <c r="I4" s="7">
         <f>B2/I2</f>
-        <v>7.336495163183832</v>
+        <v>7.7533863664826148</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1685,31 +1685,31 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7">
         <f t="shared" ref="C5:I5" si="1">(1/C4-1/C1)/(1 - 1/C1)</f>
-        <v>5.9834891521977074E-3</v>
+        <v>8.904115609174923E-3</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="1"/>
-        <v>2.9628024484909584E-2</v>
+        <v>3.3764183798414556E-3</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="1"/>
-        <v>2.2066877114248633E-2</v>
+        <v>5.588957601697272E-4</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="1"/>
-        <v>1.7817035142905328E-2</v>
+        <v>2.4319453234485089E-3</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" si="1"/>
-        <v>1.412866623300566E-2</v>
+        <v>7.8319212686819521E-3</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="1"/>
-        <v>1.4994650643826614E-2</v>
+        <v>2.681961979591173E-3</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>1.2919848395063596E-2</v>
+        <v>4.5438879747063E-3</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1747,35 +1747,35 @@
       </c>
       <c r="B7">
         <f>B2/(B6 * 2^(B6 / 2))</f>
-        <v>8.0012230801582344E-10</v>
+        <v>1.2827747750282288E-9</v>
       </c>
       <c r="C7">
         <f>B7</f>
-        <v>8.0012230801582344E-10</v>
+        <v>1.2827747750282288E-9</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:I7" si="2">C7</f>
-        <v>8.0012230801582344E-10</v>
+        <v>1.2827747750282288E-9</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>8.0012230801582344E-10</v>
+        <v>1.2827747750282288E-9</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>8.0012230801582344E-10</v>
+        <v>1.2827747750282288E-9</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>8.0012230801582344E-10</v>
+        <v>1.2827747750282288E-9</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>8.0012230801582344E-10</v>
+        <v>1.2827747750282288E-9</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>8.0012230801582344E-10</v>
+        <v>1.2827747750282288E-9</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>